<commit_message>
fix: handling errors in go-s
</commit_message>
<xml_diff>
--- a/test3s.xlsx
+++ b/test3s.xlsx
@@ -2132,7 +2132,7 @@
         <v>35</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
@@ -2196,7 +2196,7 @@
         <v>43</v>
       </c>
       <c r="J8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
@@ -2420,7 +2420,7 @@
         <v>71</v>
       </c>
       <c r="J15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16">
@@ -2484,7 +2484,7 @@
         <v>79</v>
       </c>
       <c r="J17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18">
@@ -2644,7 +2644,7 @@
         <v>100</v>
       </c>
       <c r="J22" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23">
@@ -2996,7 +2996,7 @@
         <v>147</v>
       </c>
       <c r="J33" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34">
@@ -3060,7 +3060,7 @@
         <v>155</v>
       </c>
       <c r="J35" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36">
@@ -3220,7 +3220,7 @@
         <v>179</v>
       </c>
       <c r="J40" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41">
@@ -3476,7 +3476,7 @@
         <v>218</v>
       </c>
       <c r="J48" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49">
@@ -3700,7 +3700,7 @@
         <v>247</v>
       </c>
       <c r="J55" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56">
@@ -3956,7 +3956,7 @@
         <v>279</v>
       </c>
       <c r="J63" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64">
@@ -4020,7 +4020,7 @@
         <v>288</v>
       </c>
       <c r="J65" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66">
@@ -4116,7 +4116,7 @@
         <v>302</v>
       </c>
       <c r="J68" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69">
@@ -4148,7 +4148,7 @@
         <v>307</v>
       </c>
       <c r="J69" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70">
@@ -4340,7 +4340,7 @@
         <v>333</v>
       </c>
       <c r="J75" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76">
@@ -4564,7 +4564,7 @@
         <v>363</v>
       </c>
       <c r="J82" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83">
@@ -4596,7 +4596,7 @@
         <v>367</v>
       </c>
       <c r="J83" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84">
@@ -4756,7 +4756,7 @@
         <v>389</v>
       </c>
       <c r="J88" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89">
@@ -4916,7 +4916,7 @@
         <v>412</v>
       </c>
       <c r="J93" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94">
@@ -4948,7 +4948,7 @@
         <v>416</v>
       </c>
       <c r="J94" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95">
@@ -5140,7 +5140,7 @@
         <v>445</v>
       </c>
       <c r="J100" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101">
@@ -5332,7 +5332,7 @@
         <v>469</v>
       </c>
       <c r="J106" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="107">
@@ -5364,7 +5364,7 @@
         <v>473</v>
       </c>
       <c r="J107" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="108">
@@ -5396,7 +5396,7 @@
         <v>477</v>
       </c>
       <c r="J108" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="109">

</xml_diff>

<commit_message>
new config and feature with Txhash
</commit_message>
<xml_diff>
--- a/test3s.xlsx
+++ b/test3s.xlsx
@@ -67,25 +67,25 @@
     <t>HDLO+6gqDKL6E1jY/yWe9Hplo2WEmku01/xcGjkY9NVTEr68XT2ZpqZF91a1D9JbnKkJg1UuljvPQDEfKRYAitM=</t>
   </si>
   <si>
+    <t>10.05.2016</t>
+  </si>
+  <si>
+    <t>Nikita Magda</t>
+  </si>
+  <si>
+    <t>Cryptocurrencies and Distributed Systems</t>
+  </si>
+  <si>
+    <t>120bd82d7172f419e94a</t>
+  </si>
+  <si>
+    <t>120bd82d7172f419e94a36c0569d138e9b446a64fab789c568eeacd4d2caa09d</t>
+  </si>
+  <si>
+    <t>HL/S5ow1QPozfKwI1cDRfp+h8sLtxXuxGlTDhhX9Rk8OYiSML1LOd3RwysGcf0ZTK3oLyrYpOiW7SgN6uB2ZYGE=</t>
+  </si>
+  <si>
     <t>https://drive.google.com/file/d//view</t>
-  </si>
-  <si>
-    <t>10.05.2016</t>
-  </si>
-  <si>
-    <t>Nikita Magda</t>
-  </si>
-  <si>
-    <t>Cryptocurrencies and Distributed Systems</t>
-  </si>
-  <si>
-    <t>120bd82d7172f419e94a</t>
-  </si>
-  <si>
-    <t>120bd82d7172f419e94a36c0569d138e9b446a64fab789c568eeacd4d2caa09d</t>
-  </si>
-  <si>
-    <t>HL/S5ow1QPozfKwI1cDRfp+h8sLtxXuxGlTDhhX9Rk8OYiSML1LOd3RwysGcf0ZTK3oLyrYpOiW7SgN6uB2ZYGE=</t>
   </si>
   <si>
     <t>Нестеров Максим</t>
@@ -2004,50 +2004,50 @@
         <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
         <v>22</v>
       </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" t="s">
-        <v>23</v>
-      </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
         <v>25</v>
@@ -2068,18 +2068,18 @@
         <v>27</v>
       </c>
       <c r="J4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
@@ -2100,18 +2100,18 @@
         <v>31</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
         <v>33</v>
@@ -2132,18 +2132,18 @@
         <v>35</v>
       </c>
       <c r="J6" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
         <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
         <v>37</v>
@@ -2164,18 +2164,18 @@
         <v>39</v>
       </c>
       <c r="J7" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
         <v>41</v>
@@ -2201,13 +2201,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
         <v>45</v>
@@ -2228,18 +2228,18 @@
         <v>47</v>
       </c>
       <c r="J9" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
         <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
         <v>49</v>
@@ -2260,18 +2260,18 @@
         <v>51</v>
       </c>
       <c r="J10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
         <v>53</v>
@@ -2292,18 +2292,18 @@
         <v>55</v>
       </c>
       <c r="J11" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
         <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
         <v>57</v>
@@ -2324,18 +2324,18 @@
         <v>59</v>
       </c>
       <c r="J12" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
         <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
         <v>61</v>
@@ -2356,18 +2356,18 @@
         <v>63</v>
       </c>
       <c r="J13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
         <v>64</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
         <v>65</v>
@@ -2388,18 +2388,18 @@
         <v>67</v>
       </c>
       <c r="J14" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
         <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
         <v>69</v>
@@ -2420,18 +2420,18 @@
         <v>71</v>
       </c>
       <c r="J15" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
         <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" t="s">
         <v>73</v>
@@ -2452,18 +2452,18 @@
         <v>75</v>
       </c>
       <c r="J16" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
         <v>76</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" t="s">
         <v>77</v>
@@ -2484,18 +2484,18 @@
         <v>79</v>
       </c>
       <c r="J17" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>80</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" t="s">
         <v>81</v>
@@ -2516,18 +2516,18 @@
         <v>83</v>
       </c>
       <c r="J18" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>84</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" t="s">
         <v>85</v>
@@ -2548,7 +2548,7 @@
         <v>87</v>
       </c>
       <c r="J19" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20">
@@ -2559,7 +2559,7 @@
         <v>89</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" t="s">
         <v>90</v>
@@ -2580,7 +2580,7 @@
         <v>92</v>
       </c>
       <c r="J20" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21">
@@ -2591,7 +2591,7 @@
         <v>93</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" t="s">
         <v>94</v>
@@ -2612,7 +2612,7 @@
         <v>96</v>
       </c>
       <c r="J21" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22">
@@ -2623,7 +2623,7 @@
         <v>97</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" t="s">
         <v>98</v>
@@ -2644,7 +2644,7 @@
         <v>100</v>
       </c>
       <c r="J22" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23">
@@ -2655,7 +2655,7 @@
         <v>101</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D23" t="s">
         <v>102</v>
@@ -2676,7 +2676,7 @@
         <v>104</v>
       </c>
       <c r="J23" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24">
@@ -2687,7 +2687,7 @@
         <v>105</v>
       </c>
       <c r="C24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D24" t="s">
         <v>106</v>
@@ -2708,7 +2708,7 @@
         <v>108</v>
       </c>
       <c r="J24" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25">
@@ -2719,7 +2719,7 @@
         <v>110</v>
       </c>
       <c r="C25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D25" t="s">
         <v>111</v>
@@ -2740,7 +2740,7 @@
         <v>113</v>
       </c>
       <c r="J25" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26">
@@ -2751,7 +2751,7 @@
         <v>114</v>
       </c>
       <c r="C26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D26" t="s">
         <v>115</v>
@@ -2772,7 +2772,7 @@
         <v>117</v>
       </c>
       <c r="J26" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27">
@@ -2783,7 +2783,7 @@
         <v>118</v>
       </c>
       <c r="C27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D27" t="s">
         <v>119</v>
@@ -2804,7 +2804,7 @@
         <v>121</v>
       </c>
       <c r="J27" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28">
@@ -2836,7 +2836,7 @@
         <v>127</v>
       </c>
       <c r="J28" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29">
@@ -2868,7 +2868,7 @@
         <v>131</v>
       </c>
       <c r="J29" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30">
@@ -2900,7 +2900,7 @@
         <v>135</v>
       </c>
       <c r="J30" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31">
@@ -2932,7 +2932,7 @@
         <v>139</v>
       </c>
       <c r="J31" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32">
@@ -2964,7 +2964,7 @@
         <v>143</v>
       </c>
       <c r="J32" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33">
@@ -3028,7 +3028,7 @@
         <v>151</v>
       </c>
       <c r="J34" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35">
@@ -3092,7 +3092,7 @@
         <v>159</v>
       </c>
       <c r="J36" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37">
@@ -3124,7 +3124,7 @@
         <v>163</v>
       </c>
       <c r="J37" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38">
@@ -3156,7 +3156,7 @@
         <v>169</v>
       </c>
       <c r="J38" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39">
@@ -3188,7 +3188,7 @@
         <v>174</v>
       </c>
       <c r="J39" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40">
@@ -3252,7 +3252,7 @@
         <v>184</v>
       </c>
       <c r="J41" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42">
@@ -3284,7 +3284,7 @@
         <v>189</v>
       </c>
       <c r="J42" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43">
@@ -3316,7 +3316,7 @@
         <v>194</v>
       </c>
       <c r="J43" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44">
@@ -3348,7 +3348,7 @@
         <v>198</v>
       </c>
       <c r="J44" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45">
@@ -3380,7 +3380,7 @@
         <v>203</v>
       </c>
       <c r="J45" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46">
@@ -3412,7 +3412,7 @@
         <v>208</v>
       </c>
       <c r="J46" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47">
@@ -3444,7 +3444,7 @@
         <v>214</v>
       </c>
       <c r="J47" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48">
@@ -3508,7 +3508,7 @@
         <v>223</v>
       </c>
       <c r="J49" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50">
@@ -3540,7 +3540,7 @@
         <v>227</v>
       </c>
       <c r="J50" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51">
@@ -3572,7 +3572,7 @@
         <v>231</v>
       </c>
       <c r="J51" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52">
@@ -3604,7 +3604,7 @@
         <v>235</v>
       </c>
       <c r="J52" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="53">
@@ -3636,7 +3636,7 @@
         <v>239</v>
       </c>
       <c r="J53" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="54">
@@ -3668,7 +3668,7 @@
         <v>243</v>
       </c>
       <c r="J54" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55">
@@ -3732,7 +3732,7 @@
         <v>251</v>
       </c>
       <c r="J56" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="57">
@@ -3764,7 +3764,7 @@
         <v>223</v>
       </c>
       <c r="J57" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58">
@@ -3796,7 +3796,7 @@
         <v>255</v>
       </c>
       <c r="J58" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="59">
@@ -3828,7 +3828,7 @@
         <v>260</v>
       </c>
       <c r="J59" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="60">
@@ -3860,7 +3860,7 @@
         <v>265</v>
       </c>
       <c r="J60" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61">
@@ -3892,7 +3892,7 @@
         <v>269</v>
       </c>
       <c r="J61" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="62">
@@ -3924,7 +3924,7 @@
         <v>274</v>
       </c>
       <c r="J62" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="63">
@@ -3988,7 +3988,7 @@
         <v>284</v>
       </c>
       <c r="J64" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="65">
@@ -4020,7 +4020,7 @@
         <v>288</v>
       </c>
       <c r="J65" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="66">
@@ -4052,7 +4052,7 @@
         <v>293</v>
       </c>
       <c r="J66" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="67">
@@ -4084,7 +4084,7 @@
         <v>297</v>
       </c>
       <c r="J67" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="68">
@@ -4116,7 +4116,7 @@
         <v>302</v>
       </c>
       <c r="J68" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="69">
@@ -4148,7 +4148,7 @@
         <v>307</v>
       </c>
       <c r="J69" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="70">
@@ -4180,7 +4180,7 @@
         <v>311</v>
       </c>
       <c r="J70" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="71">
@@ -4212,7 +4212,7 @@
         <v>315</v>
       </c>
       <c r="J71" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72">
@@ -4244,7 +4244,7 @@
         <v>319</v>
       </c>
       <c r="J72" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="73">
@@ -4276,7 +4276,7 @@
         <v>324</v>
       </c>
       <c r="J73" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="74">
@@ -4308,7 +4308,7 @@
         <v>328</v>
       </c>
       <c r="J74" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="75">
@@ -4340,7 +4340,7 @@
         <v>333</v>
       </c>
       <c r="J75" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="76">
@@ -4372,7 +4372,7 @@
         <v>337</v>
       </c>
       <c r="J76" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="77">
@@ -4404,7 +4404,7 @@
         <v>341</v>
       </c>
       <c r="J77" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78">
@@ -4436,7 +4436,7 @@
         <v>346</v>
       </c>
       <c r="J78" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="79">
@@ -4468,7 +4468,7 @@
         <v>350</v>
       </c>
       <c r="J79" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="80">
@@ -4500,7 +4500,7 @@
         <v>354</v>
       </c>
       <c r="J80" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="81">
@@ -4532,7 +4532,7 @@
         <v>358</v>
       </c>
       <c r="J81" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="82">
@@ -4596,7 +4596,7 @@
         <v>367</v>
       </c>
       <c r="J83" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="84">
@@ -4628,7 +4628,7 @@
         <v>371</v>
       </c>
       <c r="J84" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="85">
@@ -4660,7 +4660,7 @@
         <v>376</v>
       </c>
       <c r="J85" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="86">
@@ -4692,7 +4692,7 @@
         <v>380</v>
       </c>
       <c r="J86" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87">
@@ -4724,7 +4724,7 @@
         <v>384</v>
       </c>
       <c r="J87" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="88">
@@ -4788,7 +4788,7 @@
         <v>393</v>
       </c>
       <c r="J89" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="90">
@@ -4820,7 +4820,7 @@
         <v>398</v>
       </c>
       <c r="J90" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="91">
@@ -4852,7 +4852,7 @@
         <v>403</v>
       </c>
       <c r="J91" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="92">
@@ -4884,7 +4884,7 @@
         <v>407</v>
       </c>
       <c r="J92" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93">
@@ -4916,7 +4916,7 @@
         <v>412</v>
       </c>
       <c r="J93" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="94">
@@ -4948,7 +4948,7 @@
         <v>416</v>
       </c>
       <c r="J94" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="95">
@@ -4980,7 +4980,7 @@
         <v>421</v>
       </c>
       <c r="J95" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="96">
@@ -5012,7 +5012,7 @@
         <v>425</v>
       </c>
       <c r="J96" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="97">
@@ -5044,7 +5044,7 @@
         <v>429</v>
       </c>
       <c r="J97" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98">
@@ -5076,7 +5076,7 @@
         <v>434</v>
       </c>
       <c r="J98" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99">
@@ -5108,7 +5108,7 @@
         <v>440</v>
       </c>
       <c r="J99" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100">
@@ -5140,7 +5140,7 @@
         <v>445</v>
       </c>
       <c r="J100" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="101">
@@ -5172,7 +5172,7 @@
         <v>449</v>
       </c>
       <c r="J101" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="102">
@@ -5204,7 +5204,7 @@
         <v>453</v>
       </c>
       <c r="J102" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="103">
@@ -5236,7 +5236,7 @@
         <v>457</v>
       </c>
       <c r="J103" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="104">
@@ -5268,7 +5268,7 @@
         <v>461</v>
       </c>
       <c r="J104" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105">
@@ -5300,7 +5300,7 @@
         <v>465</v>
       </c>
       <c r="J105" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="106">
@@ -5428,7 +5428,7 @@
         <v>481</v>
       </c>
       <c r="J109" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="110">
@@ -5460,7 +5460,7 @@
         <v>485</v>
       </c>
       <c r="J110" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="111">
@@ -5492,7 +5492,7 @@
         <v>488</v>
       </c>
       <c r="J111" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="112">
@@ -5524,7 +5524,7 @@
         <v>493</v>
       </c>
       <c r="J112" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="113">
@@ -5556,7 +5556,7 @@
         <v>497</v>
       </c>
       <c r="J113" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="114">
@@ -5588,7 +5588,7 @@
         <v>500</v>
       </c>
       <c r="J114" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115">
@@ -5620,7 +5620,7 @@
         <v>503</v>
       </c>
       <c r="J115" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="116">
@@ -5652,7 +5652,7 @@
         <v>507</v>
       </c>
       <c r="J116" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="117">
@@ -5684,7 +5684,7 @@
         <v>511</v>
       </c>
       <c r="J117" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="118">
@@ -5716,7 +5716,7 @@
         <v>515</v>
       </c>
       <c r="J118" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="119">
@@ -5748,7 +5748,7 @@
         <v>519</v>
       </c>
       <c r="J119" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="120">
@@ -5780,7 +5780,7 @@
         <v>523</v>
       </c>
       <c r="J120" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="121">
@@ -5812,7 +5812,7 @@
         <v>528</v>
       </c>
       <c r="J121" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="122">
@@ -5844,7 +5844,7 @@
         <v>532</v>
       </c>
       <c r="J122" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="123">
@@ -5876,7 +5876,7 @@
         <v>536</v>
       </c>
       <c r="J123" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="124">
@@ -5908,7 +5908,7 @@
         <v>539</v>
       </c>
       <c r="J124" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>